<commit_message>
Form_EncodageFactures terminée, il manque encore que je débugge l'insertion dans la db. Il y a de nouveaux objets.
</commit_message>
<xml_diff>
--- a/ProjetCantine/bin/Debug/Resources/Facture.xlsx
+++ b/ProjetCantine/bin/Debug/Resources/Facture.xlsx
@@ -5,23 +5,23 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BDD\Factures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Source\Repos\Cantine2\ProjetCantine\bin\Debug\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14715" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Réf.</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Prix Unitaire</t>
   </si>
   <si>
-    <t>TVA %</t>
-  </si>
-  <si>
     <t>N° facture</t>
   </si>
   <si>
@@ -65,12 +62,6 @@
     <t>Total HT</t>
   </si>
   <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>Base</t>
-  </si>
-  <si>
     <t>IBAN</t>
   </si>
   <si>
@@ -78,9 +69,6 @@
   </si>
   <si>
     <t xml:space="preserve">Mode de paiement : </t>
-  </si>
-  <si>
-    <t>virement</t>
   </si>
   <si>
     <t xml:space="preserve">Période </t>
@@ -95,9 +83,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -345,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -383,9 +372,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -407,14 +393,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -422,47 +441,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,7 +532,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -817,440 +818,488 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G50"/>
+  <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22:G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
-    </row>
-    <row r="4" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="42"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="44"/>
-    </row>
-    <row r="5" spans="4:6" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37"/>
+    </row>
+    <row r="5" spans="1:6" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
       <c r="D7" s="16"/>
       <c r="E7" s="17"/>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
       <c r="D8" s="8"/>
       <c r="E8" s="6"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
       <c r="D9" s="10"/>
       <c r="E9" s="7"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="4:6" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
       <c r="D10" s="12"/>
       <c r="E10" s="7"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
       <c r="D11" s="12"/>
       <c r="E11" s="7"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="4:6" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
       <c r="D12" s="12"/>
       <c r="E12" s="7"/>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
       <c r="D13" s="12"/>
       <c r="E13" s="7"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="4:6" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
       <c r="D14" s="13"/>
       <c r="E14" s="14"/>
       <c r="F14" s="15"/>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
+    </row>
     <row r="17" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="26">
-        <f>EDATE(E7,1)</f>
-        <v>31</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C18" s="25"/>
     </row>
     <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="27"/>
+        <v>16</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="26"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="45"/>
+      <c r="C21" s="38"/>
       <c r="D21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="F21" s="2"/>
       <c r="G21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>1</v>
-      </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20">
-        <v>5</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="30"/>
       <c r="F22" s="19"/>
-      <c r="G22" s="20">
-        <f t="shared" ref="G22:G25" si="0">D22*E22</f>
-        <v>0</v>
+      <c r="G22" s="48" t="str">
+        <f>IF(ISBLANK(E22),"",D22*E22)</f>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>2</v>
-      </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20">
-        <v>6.5</v>
-      </c>
+      <c r="A23" s="3"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="30"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="G23" s="48" t="str">
+        <f t="shared" ref="G23:G38" si="0">IF(ISBLANK(E23),"",D23*E23)</f>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>3</v>
-      </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20">
-        <v>3</v>
-      </c>
+      <c r="A24" s="3"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="30"/>
       <c r="F24" s="19"/>
-      <c r="G24" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="G24" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>4</v>
-      </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20">
-        <v>1</v>
-      </c>
+      <c r="A25" s="3"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="30"/>
       <c r="F25" s="19"/>
-      <c r="G25" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="G25" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="30"/>
       <c r="F26" s="19"/>
-      <c r="G26" s="20"/>
+      <c r="G26" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="30"/>
       <c r="F27" s="19"/>
-      <c r="G27" s="20"/>
+      <c r="G27" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="30"/>
       <c r="F28" s="19"/>
-      <c r="G28" s="20"/>
+      <c r="G28" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="30"/>
       <c r="F29" s="19"/>
-      <c r="G29" s="20"/>
+      <c r="G29" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="30"/>
       <c r="F30" s="19"/>
-      <c r="G30" s="20"/>
+      <c r="G30" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="30"/>
       <c r="F31" s="19"/>
-      <c r="G31" s="20"/>
+      <c r="G31" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="30"/>
       <c r="F32" s="19"/>
-      <c r="G32" s="20"/>
+      <c r="G32" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="30"/>
       <c r="F33" s="19"/>
-      <c r="G33" s="20"/>
+      <c r="G33" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="30"/>
       <c r="F34" s="19"/>
-      <c r="G34" s="20"/>
+      <c r="G34" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="30"/>
       <c r="F35" s="19"/>
-      <c r="G35" s="20"/>
+      <c r="G35" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="30"/>
       <c r="F36" s="19"/>
-      <c r="G36" s="20"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="30"/>
       <c r="F37" s="19"/>
-      <c r="G37" s="20"/>
+      <c r="G37" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="46"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="32">
-        <f>SUM(G22:G37)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="36"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D39" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="39"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="49">
+        <f>SUM(G22:G38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
-      <c r="B40" s="21">
-        <f>G38</f>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="50"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="39"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="49"/>
+    </row>
+    <row r="42" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="41"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="51"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D43" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="42"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="52">
+        <f>G39+G41</f>
         <v>0</v>
       </c>
-      <c r="C40" s="21">
-        <f>B40*(A40/100)</f>
-        <v>0</v>
-      </c>
-      <c r="D40" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="46"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="32">
-        <f>C40</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="33"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D42" s="49" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42" s="49"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="31">
-        <f>G38+G40</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D43" s="49"/>
-      <c r="E43" s="49"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="31"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
+    </row>
+    <row r="44" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="52"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G45" s="53"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22"/>
+      <c r="A47" s="21"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="E48" s="23"/>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
+      <c r="A48" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
+      <c r="A49" s="24" t="s">
+        <v>14</v>
+      </c>
       <c r="B49" s="22"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="24" t="s">
+        <v>14</v>
+      </c>
       <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="24"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
+      <c r="A50" s="21"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="23"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="28">
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="F43:F44"/>
     <mergeCell ref="D3:F4"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D38:E39"/>
-    <mergeCell ref="D40:E41"/>
-    <mergeCell ref="D42:E43"/>
+    <mergeCell ref="D39:E40"/>
+    <mergeCell ref="D41:E42"/>
+    <mergeCell ref="D43:E44"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
@@ -1262,17 +1311,6 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1286,7 +1324,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1299,7 +1337,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>